<commit_message>
meter updates, DFM updates
</commit_message>
<xml_diff>
--- a/Mechanical/Design Memos/costed parts list.xlsx
+++ b/Mechanical/Design Memos/costed parts list.xlsx
@@ -1017,221 +1017,12 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4B61F568-99D0-4821-AC24-42F3DACD7731}" diskRevisions="1" revisionId="25" version="3">
-  <header guid="{A6DD73F5-2278-4923-99AD-287DFAA36843}" dateTime="2014-11-23T22:49:11" maxSheetId="2" userName="Sam Feller" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{77A8C7E2-EE07-4F44-B347-31477F0B70CC}" dateTime="2014-11-23T23:01:39" maxSheetId="2" userName="Sam Feller" r:id="rId2" minRId="1" maxRId="23">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{4B61F568-99D0-4821-AC24-42F3DACD7731}" dateTime="2014-11-24T11:17:57" maxSheetId="2" userName="Sam Feller" r:id="rId3" minRId="24" maxRId="25">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="1">
-    <nc r="U1" t="inlineStr">
-      <is>
-        <t>EXTENDED COST</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="U1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Century Gothic"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="2" sId="1">
-    <nc r="U2">
-      <f>E2*P2</f>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="1">
-    <nc r="U4">
-      <f>E4*P4</f>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="1">
-    <nc r="U5">
-      <f>E5*P5</f>
-    </nc>
-  </rcc>
-  <rcc rId="5" sId="1">
-    <nc r="U6">
-      <f>E6*P6</f>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="1">
-    <nc r="U7">
-      <f>E7*P7</f>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="1">
-    <nc r="U8">
-      <f>E8*P8</f>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="1">
-    <nc r="U9">
-      <f>E9*P9</f>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="1">
-    <nc r="U10">
-      <f>E10*P10</f>
-    </nc>
-  </rcc>
-  <rcc rId="10" sId="1">
-    <nc r="U13">
-      <f>SUM(U2:U10)</f>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="1">
-    <nc r="T13" t="inlineStr">
-      <is>
-        <t>BASIC COGS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T13:U13" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="12" sId="1">
-    <nc r="T15" t="inlineStr">
-      <is>
-        <t>COGS @QTY100</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="13" sId="1">
-    <nc r="U15">
-      <f>U13*100</f>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T15:U15" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rrc rId="14" sId="1" eol="1" ref="A16:XFD16" action="insertRow"/>
-  <rcc rId="15" sId="1">
-    <nc r="T16" t="inlineStr">
-      <is>
-        <t>TOOLING COST</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="1">
-    <nc r="U16">
-      <f>SUM(Q2:Q10)</f>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T16:U16" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rrc rId="17" sId="1" eol="1" ref="A17:XFD17" action="insertRow"/>
-  <rcc rId="18" sId="1">
-    <nc r="T17" t="inlineStr">
-      <is>
-        <t>MINIMUM BREAK EVEN</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Source Code Pro"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rm rId="19" sheetId="1" source="T17" destination="T20" sourceSheetId="1"/>
-  <rrc rId="20" sId="1" eol="1" ref="A17:XFD17" action="insertRow"/>
-  <rcc rId="21" sId="1">
-    <nc r="T17" t="inlineStr">
-      <is>
-        <t>reverse 10% kickstarter</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Source Code Pro"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="22" sId="1">
-    <nc r="U17">
-      <f>(SUM(U15:U16)/90)*100-SUM(U15:U16)</f>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="1">
-    <nc r="U21">
-      <f>SUM(U15:U17)</f>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
backer updates and artwork changes
</commit_message>
<xml_diff>
--- a/Mechanical/Design Memos/costed parts list.xlsx
+++ b/Mechanical/Design Memos/costed parts list.xlsx
@@ -1017,221 +1017,12 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4B61F568-99D0-4821-AC24-42F3DACD7731}" diskRevisions="1" revisionId="25" version="3">
-  <header guid="{A6DD73F5-2278-4923-99AD-287DFAA36843}" dateTime="2014-11-23T22:49:11" maxSheetId="2" userName="Sam Feller" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{77A8C7E2-EE07-4F44-B347-31477F0B70CC}" dateTime="2014-11-23T23:01:39" maxSheetId="2" userName="Sam Feller" r:id="rId2" minRId="1" maxRId="23">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
   <header guid="{4B61F568-99D0-4821-AC24-42F3DACD7731}" dateTime="2014-11-24T11:17:57" maxSheetId="2" userName="Sam Feller" r:id="rId3" minRId="24" maxRId="25">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="1">
-    <nc r="U1" t="inlineStr">
-      <is>
-        <t>EXTENDED COST</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="U1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Century Gothic"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="2" sId="1">
-    <nc r="U2">
-      <f>E2*P2</f>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="1">
-    <nc r="U4">
-      <f>E4*P4</f>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="1">
-    <nc r="U5">
-      <f>E5*P5</f>
-    </nc>
-  </rcc>
-  <rcc rId="5" sId="1">
-    <nc r="U6">
-      <f>E6*P6</f>
-    </nc>
-  </rcc>
-  <rcc rId="6" sId="1">
-    <nc r="U7">
-      <f>E7*P7</f>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="1">
-    <nc r="U8">
-      <f>E8*P8</f>
-    </nc>
-  </rcc>
-  <rcc rId="8" sId="1">
-    <nc r="U9">
-      <f>E9*P9</f>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="1">
-    <nc r="U10">
-      <f>E10*P10</f>
-    </nc>
-  </rcc>
-  <rcc rId="10" sId="1">
-    <nc r="U13">
-      <f>SUM(U2:U10)</f>
-    </nc>
-  </rcc>
-  <rcc rId="11" sId="1">
-    <nc r="T13" t="inlineStr">
-      <is>
-        <t>BASIC COGS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T13:U13" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="12" sId="1">
-    <nc r="T15" t="inlineStr">
-      <is>
-        <t>COGS @QTY100</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="13" sId="1">
-    <nc r="U15">
-      <f>U13*100</f>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T15:U15" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rrc rId="14" sId="1" eol="1" ref="A16:XFD16" action="insertRow"/>
-  <rcc rId="15" sId="1">
-    <nc r="T16" t="inlineStr">
-      <is>
-        <t>TOOLING COST</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="16" sId="1">
-    <nc r="U16">
-      <f>SUM(Q2:Q10)</f>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T16:U16" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rrc rId="17" sId="1" eol="1" ref="A17:XFD17" action="insertRow"/>
-  <rcc rId="18" sId="1">
-    <nc r="T17" t="inlineStr">
-      <is>
-        <t>MINIMUM BREAK EVEN</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Source Code Pro"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rm rId="19" sheetId="1" source="T17" destination="T20" sourceSheetId="1"/>
-  <rrc rId="20" sId="1" eol="1" ref="A17:XFD17" action="insertRow"/>
-  <rcc rId="21" sId="1">
-    <nc r="T17" t="inlineStr">
-      <is>
-        <t>reverse 10% kickstarter</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="T17">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Source Code Pro"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="22" sId="1">
-    <nc r="U17">
-      <f>(SUM(U15:U16)/90)*100-SUM(U15:U16)</f>
-    </nc>
-  </rcc>
-  <rcc rId="23" sId="1">
-    <nc r="U21">
-      <f>SUM(U15:U17)</f>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>